<commit_message>
Finish experiments prompt grok
</commit_message>
<xml_diff>
--- a/out/metadata_camembert.xlsx
+++ b/out/metadata_camembert.xlsx
@@ -473,27 +473,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>24EM03308</t>
+          <t>24EM03355</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18/07/24</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Adénocarcinome pulmonaire</t>
+          <t>cancer pulmonaire</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CMP</t>
+          <t>CurePath</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Adénocarcinome pulmonaire</t>
+          <t>Carcinome non à petites cellules NOS</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -503,34 +503,34 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>24EM03308</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24EM04107</t>
+          <t>24EM03456</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>24CU062294-1</t>
+          <t>24CU052383</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15:35</t>
+          <t>COSMIC</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CurePath</t>
+          <t>Curepath</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PF1 oncocytaire</t>
+          <t>Adénocarcinome TTF1+</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,34 +540,34 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>24EM04107</t>
+          <t>&lt;10%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24EM03462</t>
+          <t>24EM03461</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24219576</t>
+          <t>24CU002162-4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Foie</t>
+          <t>Adénocarcinome colorectal métastatique</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CMP</t>
+          <t>Adénocarcinome colorectal métastatique</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Métastase hépatique d’un adénocarcinome mammaire</t>
+          <t>Adénocarcinome colorectal métastatique</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -577,34 +577,34 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>24EM03462</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>24EM04099</t>
+          <t>24EM03462</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PF1</t>
+          <t>24219576</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>frottis2</t>
+          <t>adénocarcinome mammaire</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CurePath</t>
+          <t>CMP</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>PF1</t>
+          <t>Métastase hépatique d’un adénocarcinome mammaire</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -614,222 +614,222 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>24EM04099</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>24EM03839</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>24EC09559</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20cytologie</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Erasme</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>PF2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>3 / 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>24EM04099</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PF1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>THYROID CANCER</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CurePath</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>PF1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>3 / 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>24EM04107</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>24CU062294-1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>thyroïdiens</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>CurePath</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>PF1 oncocytaire</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>10%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>24EM04337</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8, 10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>lymphomes, des cancers du sein ou d'autres cancers solides</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CMP Pathology</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>masse gastrique</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>38%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>24EM04347</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>23CU032757-1.02</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>carcinome urothélial invasif</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>carcinome urothélial invasif</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>carcinome urothélial invasif</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Optimale</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>18, 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>24EM03451</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>24BB11466 07</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Tumeur de la granulosa</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>tumeurs de l’ovaire, de
 l’endomètre et du sein</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Tumeur de la granulosa</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Optimale</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>24EM03451</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>24EM04347</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>23CU032757-1.02</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>carcinome urothélial invasif</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>carcinome urothélial invasif</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>carcinome urothélial invasif</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Optimale</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>24EM04347</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>24EM03355</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Carcinome non à petites cellules NOS</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>CurePath</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Carcinome non à petites cellules NOS</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Optimale</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>24EM03355</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>24EM03461</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>24CU002162-4</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Adénocarcinome colorectal métastatique</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Adénocarcinome colorectal métastatique</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Adénocarcinome colorectal métastatique</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Optimale</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>24EM03461</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>24EM03352</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>24MH9794</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Adénocarcinome lieberkühnien</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Centre Hospitalier de Mouscron</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Adénocarcinome lieberkühnien</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Optimale</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>24EM03352</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>24EM03460</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>24MH9721</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Adénocarcinome lieberkühnien</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Centre Hospitalier de Mouscron</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Adénocarcinome lieberkühnien</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Optimale</t>
@@ -837,35 +837,34 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>24EM03460</t>
+          <t>25%</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>24EM03839</t>
+          <t>24EM03460</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>24EC09559</t>
+          <t>24MH9721</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>zones
-tumorales</t>
+          <t>COLON &amp; LUNG CANCER</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Erasme</t>
+          <t>Centre Hospitalier de Mouscron</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>PF2</t>
+          <t>Adénocarcinome lieberkühnien</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -882,27 +881,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>24EM04337</t>
+          <t>24EM03308</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8, 10</t>
+          <t>18/07/24</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>masse gastrique</t>
+          <t>Adénocarcinome pulmonaire</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CMP Pathology</t>
+          <t>CMP</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>masse gastrique</t>
+          <t>Adénocarcinome pulmonaire</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -912,35 +911,34 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>24EM04337</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>24EM03456</t>
+          <t>24EM03352</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>24CU052383</t>
+          <t>24MH9794</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>zones
-tumorales</t>
+          <t>COLON &amp; LUNG CANCER</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Curepath</t>
+          <t>Centre Hospitalier de Mouscron</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Adénocarcinome TTF1+</t>
+          <t>Adénocarcinome lieberkühnien</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -950,7 +948,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>24EM03456</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
first part of prompt design results done
</commit_message>
<xml_diff>
--- a/out/metadata_camembert.xlsx
+++ b/out/metadata_camembert.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Qualité du séquencage</t>
+          <t>Qualité du séquençage</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -473,27 +473,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>24EM03355</t>
+          <t>24EM03308</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>18/07/24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>cancer pulmonaire</t>
+          <t>Adénocarcinome pulmonaire</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CurePath</t>
+          <t>CMP</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Carcinome non à petites cellules NOS</t>
+          <t>Adénocarcinome pulmonaire</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -510,27 +510,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>24EM03456</t>
+          <t>24EM04107</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>24CU052383</t>
+          <t>24CU062294-1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>COSMIC</t>
+          <t>thyroïdiens</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Curepath</t>
+          <t>CurePath</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Adénocarcinome TTF1+</t>
+          <t>PF1 oncocytaire</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -540,34 +540,34 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>&lt;10%</t>
+          <t>10%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>24EM03461</t>
+          <t>24EM03462</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24CU002162-4</t>
+          <t>24219576</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Adénocarcinome colorectal métastatique</t>
+          <t>adénocarcinome mammaire</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Adénocarcinome colorectal métastatique</t>
+          <t>CMP</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Adénocarcinome colorectal métastatique</t>
+          <t>Métastase hépatique d’un adénocarcinome mammaire</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -584,27 +584,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>24EM03462</t>
+          <t>24EM04099</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24219576</t>
+          <t>PF1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>adénocarcinome mammaire</t>
+          <t>THYROID CANCER</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CMP</t>
+          <t>CurePath</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Métastase hépatique d’un adénocarcinome mammaire</t>
+          <t>PF1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -621,27 +621,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>24EM03839</t>
+          <t>24EM03451</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24EC09559</t>
+          <t>24BB11466 07</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>20cytologie</t>
+          <t>Tumeur de la granulosa</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Erasme</t>
+          <t>tumeurs de l’ovaire, de
+l’endomètre et du sein</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>PF2</t>
+          <t>Tumeur de la granulosa</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -651,34 +652,34 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3 / 3</t>
+          <t>25%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>24EM04099</t>
+          <t>24EM04347</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PF1</t>
+          <t>23CU032757-1.02</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>THYROID CANCER</t>
+          <t>carcinome urothélial invasif</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CurePath</t>
+          <t>carcinome urothélial invasif</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PF1</t>
+          <t>carcinome urothélial invasif</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -688,24 +689,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3 / 3</t>
+          <t>18, 20</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>24EM04107</t>
+          <t>24EM03355</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>24CU062294-1</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>thyroïdiens</t>
+          <t>cancer pulmonaire</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -715,7 +716,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PF1 oncocytaire</t>
+          <t>Carcinome non à petites cellules NOS</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -725,34 +726,34 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>10%</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>24EM04337</t>
+          <t>24EM03461</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8, 10</t>
+          <t>24CU002162-4</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>lymphomes, des cancers du sein ou d'autres cancers solides</t>
+          <t>Adénocarcinome colorectal métastatique</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>CMP Pathology</t>
+          <t>Adénocarcinome colorectal métastatique</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>masse gastrique</t>
+          <t>Adénocarcinome colorectal métastatique</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -762,34 +763,34 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>38%</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>24EM04347</t>
+          <t>24EM03352</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23CU032757-1.02</t>
+          <t>24MH9794</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>carcinome urothélial invasif</t>
+          <t>COLON &amp; LUNG CANCER</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>carcinome urothélial invasif</t>
+          <t>Centre Hospitalier de Mouscron</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>carcinome urothélial invasif</t>
+          <t>Adénocarcinome lieberkühnien</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -799,35 +800,34 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>18, 20</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>24EM03451</t>
+          <t>24EM03460</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24BB11466 07</t>
+          <t>24MH9721</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tumeur de la granulosa</t>
+          <t>COLON &amp; LUNG CANCER</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>tumeurs de l’ovaire, de
-l’endomètre et du sein</t>
+          <t>Centre Hospitalier de Mouscron</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Tumeur de la granulosa</t>
+          <t>Adénocarcinome lieberkühnien</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -837,34 +837,34 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>3 / 3</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>24EM03460</t>
+          <t>24EM03839</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>24MH9721</t>
+          <t>24EC09559</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>COLON &amp; LUNG CANCER</t>
+          <t>20cytologie</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Centre Hospitalier de Mouscron</t>
+          <t>Erasme</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Adénocarcinome lieberkühnien</t>
+          <t>PF2</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -881,27 +881,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>24EM03308</t>
+          <t>24EM04337</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>18/07/24</t>
+          <t>8, 10</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Adénocarcinome pulmonaire</t>
+          <t>lymphomes, des cancers du sein ou d'autres cancers solides</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CMP</t>
+          <t>CMP Pathology</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Adénocarcinome pulmonaire</t>
+          <t>masse gastrique</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -911,34 +911,34 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>3 / 3</t>
+          <t>38%</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>24EM03352</t>
+          <t>24EM03456</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>24MH9794</t>
+          <t>24CU052383</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>COLON &amp; LUNG CANCER</t>
+          <t>COSMIC</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Centre Hospitalier de Mouscron</t>
+          <t>Curepath</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Adénocarcinome lieberkühnien</t>
+          <t>Adénocarcinome TTF1+</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -948,7 +948,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>3 / 3</t>
+          <t>&lt;10%</t>
         </is>
       </c>
     </row>

</xml_diff>